<commit_message>
Added Members Collect method
</commit_message>
<xml_diff>
--- a/TimeKeeperStatuses.xlsx
+++ b/TimeKeeperStatuses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\TimeKeeper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABD0E80-50D4-4DC7-BA45-ED67B49ED86A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DF40F4-4762-42AB-A7DF-8427F828CF09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="828" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployeePosition" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Id</t>
   </si>
@@ -160,7 +160,13 @@
     <t>Fixed bid</t>
   </si>
   <si>
-    <t>???</t>
+    <t>Hourly</t>
+  </si>
+  <si>
+    <t>PerCapita</t>
+  </si>
+  <si>
+    <t>ProBono</t>
   </si>
 </sst>
 </file>
@@ -475,7 +481,7 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -806,8 +812,8 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
@@ -841,7 +847,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -849,7 +855,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added MemberStatus table, implemented all relations in repositories, unit of work, seed methods etc
</commit_message>
<xml_diff>
--- a/TimeKeeperStatuses.xlsx
+++ b/TimeKeeperStatuses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\TimeKeeper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DF40F4-4762-42AB-A7DF-8427F828CF09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A801DC5-B37A-4BC5-B371-578C3E895BF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="828" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="828" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployeePosition" sheetId="10" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="CustomerStatus" sheetId="13" r:id="rId4"/>
     <sheet name="ProjectStatus" sheetId="14" r:id="rId5"/>
     <sheet name="PricingStatus" sheetId="15" r:id="rId6"/>
+    <sheet name="MemberStatus" sheetId="16" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Calendar">#REF!</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Id</t>
   </si>
@@ -167,6 +168,9 @@
   </si>
   <si>
     <t>ProBono</t>
+  </si>
+  <si>
+    <t>Waiting for the task</t>
   </si>
 </sst>
 </file>
@@ -812,8 +816,8 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
@@ -864,4 +868,59 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC990A93-C9C7-49C5-8679-D00808C32B95}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>